<commit_message>
Added temporary mute permissions and commands for bot.
</commit_message>
<xml_diff>
--- a/denconvert.xlsx
+++ b/denconvert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prisc\Documents\raidhelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136AEF9B-6D86-43E7-8A34-471F9626078F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073E9FF4-35E3-4088-A560-5DB4187D634C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6456" yWindow="3540" windowWidth="16584" windowHeight="9420" xr2:uid="{AE9E47E1-5B87-41CD-968F-BA62D4A7B757}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{AE9E47E1-5B87-41CD-968F-BA62D4A7B757}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CD8A54-E436-4D45-9056-35248B7FE0CB}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,7 +2357,7 @@
         <v>17</v>
       </c>
       <c r="D72" s="4">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>170</v>
@@ -2391,7 +2391,7 @@
         <v>15</v>
       </c>
       <c r="D74" s="4">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>170</v>

</xml_diff>